<commit_message>
Added routine to compress the DBs
</commit_message>
<xml_diff>
--- a/backupParameters_example.xlsx
+++ b/backupParameters_example.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Team\Crow\_Python\SDEbackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2DE80DE7-5D70-4F11-9963-F26452B57894}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0A81446-2645-4EA1-B665-A3F0B522AEBD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9555" windowHeight="2385" xr2:uid="{F0A731C3-9B6C-4667-9ECD-D5A3BCDB48BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9555" windowHeight="2385" activeTab="3" xr2:uid="{F0A731C3-9B6C-4667-9ECD-D5A3BCDB48BF}"/>
   </bookViews>
   <sheets>
     <sheet name="dbs" sheetId="1" r:id="rId1"/>
     <sheet name="email" sheetId="2" r:id="rId2"/>
+    <sheet name="sde" sheetId="3" r:id="rId3"/>
+    <sheet name="emailRecipient" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>SDE_server</t>
   </si>
@@ -83,6 +85,21 @@
   </si>
   <si>
     <t>application specific password</t>
+  </si>
+  <si>
+    <t>sde</t>
+  </si>
+  <si>
+    <t>*&amp;^%#^&amp;!!</t>
+  </si>
+  <si>
+    <t>emailAddresses</t>
+  </si>
+  <si>
+    <t>AZLsaksjd@gmail.com</t>
+  </si>
+  <si>
+    <t>sdajdadkjhs@usgs.gov</t>
   </si>
 </sst>
 </file>
@@ -446,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AEC987-AA9D-497D-B499-5FA1301BC253}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -537,7 +554,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,4 +582,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BEBE65-95AA-4065-B013-890534F17209}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717DBB0A-594E-4144-83AC-99AD5D1C509D}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>